<commit_message>
Audit biomass sample C/N aggregated data set
Annotate deviations, resolve existing discrepancies, clearly mark
remaining discrepancies, verify data against original sources,
implement standard aggregation method, and conduct statistical
analysis on burn vs. non-burn data from 2014 at MMTN
</commit_message>
<xml_diff>
--- a/analysis/Impact of fire at MMTN.xlsx
+++ b/analysis/Impact of fire at MMTN.xlsx
@@ -5,17 +5,19 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2011 REACCH\2011-reacch-biomass.git\records\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2011 REACCH\2011-reacch-biomass.git\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11415"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11415" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Above-ground biomass" sheetId="1" r:id="rId1"/>
+    <sheet name="C-N content" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Above-ground biomass'!$A:$D</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'C-N content'!$A:$F</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="24">
   <si>
     <t>t Critical two-tail</t>
   </si>
@@ -109,12 +111,49 @@
 Post-burn
 Analysis</t>
   </si>
+  <si>
+    <t>Carbon</t>
+  </si>
+  <si>
+    <t>Nitrogen</t>
+  </si>
+  <si>
+    <t>2014-08-06
+product (grain)
+(suspect point omitted)</t>
+  </si>
+  <si>
+    <t>2014-08-06
+field residue
+(suspect point omitted)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Several samples demonstate statistically significant differences in nitrogen or carbon 
+content in burned vs. non-burned areas (p &lt; 0.1, 0.05, or 0.01 = 10%, 5%, 1% significance levels)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Assuming samples satisfy normal distribution)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,8 +169,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -150,8 +195,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -190,19 +253,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -214,18 +283,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -234,24 +294,65 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -538,7 +639,7 @@
   </sheetPr>
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
@@ -550,112 +651,112 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="21" t="s">
         <v>16</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="9"/>
+      <c r="D2" s="18"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="22"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8" t="s">
+      <c r="B3" s="7"/>
+      <c r="C3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="22"/>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>108</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>79.333333333333329</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="22"/>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>2122</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>394.33333333333394</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>4</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="6">
-        <v>0</v>
-      </c>
-      <c r="D7" s="6"/>
+      <c r="C7" s="5">
+        <v>0</v>
+      </c>
+      <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
-      <c r="B8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="4">
+      <c r="B8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="3">
         <v>4</v>
       </c>
-      <c r="D8" s="4"/>
+      <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <v>1.1142083934812512</v>
       </c>
-      <c r="D9" s="4"/>
+      <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>0.32762102322119468</v>
       </c>
-      <c r="D10" s="4"/>
+      <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22"/>
@@ -668,210 +769,210 @@
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="19"/>
+      <c r="D12" s="25"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18" t="s">
+      <c r="A13" s="24"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="14" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="16" t="s">
+      <c r="A14" s="24"/>
+      <c r="B14" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="16">
+      <c r="C14" s="12">
         <v>270</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="12">
         <v>224</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="16" t="s">
+      <c r="A15" s="24"/>
+      <c r="B15" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="16">
+      <c r="C15" s="12">
         <v>8323.3333333333339</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="12">
         <v>5239</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="16" t="s">
+      <c r="A16" s="24"/>
+      <c r="B16" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="16">
+      <c r="C16" s="12">
         <v>4</v>
       </c>
-      <c r="D16" s="16">
+      <c r="D16" s="12">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="16" t="s">
+      <c r="A17" s="24"/>
+      <c r="B17" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="16">
-        <v>0</v>
-      </c>
-      <c r="D17" s="16"/>
+      <c r="C17" s="12">
+        <v>0</v>
+      </c>
+      <c r="D17" s="12"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="16">
+      <c r="A18" s="24"/>
+      <c r="B18" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="12">
         <v>5</v>
       </c>
-      <c r="D18" s="16"/>
+      <c r="D18" s="12"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="16" t="s">
+      <c r="A19" s="24"/>
+      <c r="B19" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="17">
+      <c r="C19" s="13">
         <v>0.74356535074161345</v>
       </c>
-      <c r="D19" s="16"/>
+      <c r="D19" s="12"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="16" t="s">
+      <c r="A20" s="24"/>
+      <c r="B20" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="4">
         <v>0.49058151904888192</v>
       </c>
-      <c r="D20" s="16"/>
+      <c r="D20" s="12"/>
     </row>
     <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="14"/>
-      <c r="B21" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" s="12">
+      <c r="A21" s="24"/>
+      <c r="B21" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="9">
         <v>4.0321429835552278</v>
       </c>
-      <c r="D21" s="13"/>
+      <c r="D21" s="10"/>
     </row>
     <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="24" t="s">
+      <c r="A22" s="21" t="s">
         <v>14</v>
       </c>
       <c r="B22" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="9"/>
+      <c r="D22" s="18"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="22"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8" t="s">
+      <c r="B23" s="7"/>
+      <c r="C23" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="22"/>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="5">
         <v>432.75</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="5">
         <v>355.33333333333331</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="22"/>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="5">
         <v>49105.583333333336</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="5">
         <v>23433.333333333343</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="22"/>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C26" s="5">
         <v>4</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="5">
         <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="22"/>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="6">
-        <v>0</v>
-      </c>
-      <c r="D27" s="6"/>
+      <c r="C27" s="5">
+        <v>0</v>
+      </c>
+      <c r="D27" s="5"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="22"/>
-      <c r="B28" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C28" s="4">
+      <c r="B28" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="3">
         <v>5</v>
       </c>
-      <c r="D28" s="4"/>
+      <c r="D28" s="3"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="22"/>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="6">
         <v>0.5462248423366346</v>
       </c>
-      <c r="D29" s="4"/>
+      <c r="D29" s="3"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="22"/>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="23">
+      <c r="C30" s="16">
         <v>0.60839065599175624</v>
       </c>
-      <c r="D30" s="6"/>
+      <c r="D30" s="5"/>
     </row>
     <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="22"/>
@@ -884,213 +985,213 @@
       <c r="D31" s="2"/>
     </row>
     <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="21" t="s">
+      <c r="A32" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="20" t="s">
+      <c r="B32" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="19" t="s">
+      <c r="C32" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D32" s="19"/>
+      <c r="D32" s="25"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="18" t="s">
+      <c r="A33" s="24"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D33" s="18" t="s">
+      <c r="D33" s="14" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
-      <c r="B34" s="16" t="s">
+      <c r="A34" s="24"/>
+      <c r="B34" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C34" s="16">
+      <c r="C34" s="12">
         <v>290.66666666666669</v>
       </c>
-      <c r="D34" s="16">
+      <c r="D34" s="12">
         <v>183</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
-      <c r="B35" s="16" t="s">
+      <c r="A35" s="24"/>
+      <c r="B35" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C35" s="16">
+      <c r="C35" s="12">
         <v>12709.333333333328</v>
       </c>
-      <c r="D35" s="16">
+      <c r="D35" s="12">
         <v>3631</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="14"/>
-      <c r="B36" s="16" t="s">
+      <c r="A36" s="24"/>
+      <c r="B36" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C36" s="16">
-        <v>3</v>
-      </c>
-      <c r="D36" s="16">
+      <c r="C36" s="12">
+        <v>3</v>
+      </c>
+      <c r="D36" s="12">
         <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
-      <c r="B37" s="16" t="s">
+      <c r="A37" s="24"/>
+      <c r="B37" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C37" s="16">
-        <v>0</v>
-      </c>
-      <c r="D37" s="16"/>
+      <c r="C37" s="12">
+        <v>0</v>
+      </c>
+      <c r="D37" s="12"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="14"/>
-      <c r="B38" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C38" s="15">
-        <v>3</v>
-      </c>
-      <c r="D38" s="15"/>
+      <c r="A38" s="24"/>
+      <c r="B38" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="11">
+        <v>3</v>
+      </c>
+      <c r="D38" s="11"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
-      <c r="B39" s="16" t="s">
+      <c r="A39" s="24"/>
+      <c r="B39" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C39" s="17">
+      <c r="C39" s="13">
         <v>1.4588526853891466</v>
       </c>
-      <c r="D39" s="15"/>
+      <c r="D39" s="11"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="14"/>
-      <c r="B40" s="16" t="s">
+      <c r="A40" s="24"/>
+      <c r="B40" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C40" s="5">
+      <c r="C40" s="4">
         <v>0.24069621645994091</v>
       </c>
-      <c r="D40" s="15"/>
+      <c r="D40" s="11"/>
     </row>
     <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="14"/>
-      <c r="B41" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C41" s="12">
+      <c r="A41" s="24"/>
+      <c r="B41" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" s="9">
         <v>5.8409093097333571</v>
       </c>
-      <c r="D41" s="12"/>
+      <c r="D41" s="9"/>
     </row>
     <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="11" t="s">
+      <c r="A42" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="B42" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C42" s="9" t="s">
+      <c r="C42" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D42" s="9"/>
+      <c r="D42" s="18"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="3"/>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8" t="s">
+      <c r="A43" s="20"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D43" s="8" t="s">
+      <c r="D43" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
-      <c r="B44" s="6" t="s">
+      <c r="A44" s="20"/>
+      <c r="B44" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C44" s="6">
+      <c r="C44" s="5">
         <v>74.45</v>
       </c>
-      <c r="D44" s="6">
+      <c r="D44" s="5">
         <v>46.163333333333334</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="3"/>
-      <c r="B45" s="6" t="s">
+      <c r="A45" s="20"/>
+      <c r="B45" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C45" s="6">
+      <c r="C45" s="5">
         <v>1030.411900000001</v>
       </c>
-      <c r="D45" s="6">
+      <c r="D45" s="5">
         <v>413.04573333333292</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="3"/>
-      <c r="B46" s="6" t="s">
+      <c r="A46" s="20"/>
+      <c r="B46" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C46" s="6">
-        <v>3</v>
-      </c>
-      <c r="D46" s="6">
+      <c r="C46" s="5">
+        <v>3</v>
+      </c>
+      <c r="D46" s="5">
         <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="3"/>
-      <c r="B47" s="6" t="s">
+      <c r="A47" s="20"/>
+      <c r="B47" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C47" s="6">
-        <v>0</v>
-      </c>
-      <c r="D47" s="6"/>
+      <c r="C47" s="5">
+        <v>0</v>
+      </c>
+      <c r="D47" s="5"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="3"/>
-      <c r="B48" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C48" s="4">
-        <v>3</v>
-      </c>
-      <c r="D48" s="4"/>
+      <c r="A48" s="20"/>
+      <c r="B48" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48" s="3">
+        <v>3</v>
+      </c>
+      <c r="D48" s="3"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="3"/>
-      <c r="B49" s="6" t="s">
+      <c r="A49" s="20"/>
+      <c r="B49" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C49" s="7">
+      <c r="C49" s="6">
         <v>1.2895565132463891</v>
       </c>
-      <c r="D49" s="4"/>
+      <c r="D49" s="3"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="3"/>
-      <c r="B50" s="6" t="s">
+      <c r="A50" s="20"/>
+      <c r="B50" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C50" s="5">
+      <c r="C50" s="4">
         <v>0.28762692417348057</v>
       </c>
-      <c r="D50" s="4"/>
+      <c r="D50" s="3"/>
     </row>
     <row r="51" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="3"/>
+      <c r="A51" s="20"/>
       <c r="B51" s="2" t="s">
         <v>0</v>
       </c>
@@ -1101,20 +1202,933 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="A12:A21"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A2:A11"/>
     <mergeCell ref="C42:D42"/>
     <mergeCell ref="A42:A51"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="A22:A31"/>
     <mergeCell ref="A32:A41"/>
     <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="A12:A21"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A2:A11"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="87" fitToWidth="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;F&amp;C&amp;A</oddHeader>
+    <oddFooter>Page &amp;P of &amp;N</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:F56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="45.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="27"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="20"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="27"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="20"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="20"/>
+      <c r="B5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="5">
+        <v>3.0374124999999998</v>
+      </c>
+      <c r="D5" s="5">
+        <v>2.6953499999999999</v>
+      </c>
+      <c r="E5" s="5">
+        <v>44.503250000000001</v>
+      </c>
+      <c r="F5" s="5">
+        <v>43.953500000000012</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="20"/>
+      <c r="B6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="5">
+        <v>9.6421209821428558E-2</v>
+      </c>
+      <c r="D6" s="5">
+        <v>4.0996722999999999E-2</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0.39326964285714278</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0.16369190000000094</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="20"/>
+      <c r="B7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="5">
+        <v>8</v>
+      </c>
+      <c r="D7" s="5">
+        <v>6</v>
+      </c>
+      <c r="E7" s="5">
+        <v>8</v>
+      </c>
+      <c r="F7" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="20"/>
+      <c r="B8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5">
+        <v>0</v>
+      </c>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="20"/>
+      <c r="B9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="5">
+        <v>12</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5">
+        <v>12</v>
+      </c>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="20"/>
+      <c r="B10" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="37">
+        <v>2.4890976233176083</v>
+      </c>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37">
+        <v>1.9883962822155521</v>
+      </c>
+      <c r="F10" s="37"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="20"/>
+      <c r="B11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="32">
+        <v>2.8479185341295177E-2</v>
+      </c>
+      <c r="D11" s="37"/>
+      <c r="E11" s="38">
+        <v>7.0065910023593053E-2</v>
+      </c>
+      <c r="F11" s="37"/>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="20"/>
+      <c r="B12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="36">
+        <v>3.0545395893929017</v>
+      </c>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36">
+        <v>3.0545395893929017</v>
+      </c>
+      <c r="F12" s="36"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="35"/>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="24"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="34"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="24"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="24"/>
+      <c r="B16" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="30">
+        <v>2.5873374999999998</v>
+      </c>
+      <c r="D16" s="30">
+        <v>2.2740666666666667</v>
+      </c>
+      <c r="E16" s="30">
+        <v>45.106750000000005</v>
+      </c>
+      <c r="F16" s="30">
+        <v>45.134666666666668</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="24"/>
+      <c r="B17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="30">
+        <v>6.4994408392857111E-2</v>
+      </c>
+      <c r="D17" s="30">
+        <v>3.0665322666666672E-2</v>
+      </c>
+      <c r="E17" s="30">
+        <v>0.76110335714285626</v>
+      </c>
+      <c r="F17" s="30">
+        <v>0.36973346666666784</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="24"/>
+      <c r="B18" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="30">
+        <v>8</v>
+      </c>
+      <c r="D18" s="30">
+        <v>6</v>
+      </c>
+      <c r="E18" s="30">
+        <v>8</v>
+      </c>
+      <c r="F18" s="30">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="24"/>
+      <c r="B19" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="30">
+        <v>0</v>
+      </c>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30">
+        <v>0</v>
+      </c>
+      <c r="F19" s="30"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="24"/>
+      <c r="B20" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="30">
+        <v>12</v>
+      </c>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30">
+        <v>12</v>
+      </c>
+      <c r="F20" s="30"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="24"/>
+      <c r="B21" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="30">
+        <v>2.7230455267890274</v>
+      </c>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30">
+        <v>-7.0509186866482609E-2</v>
+      </c>
+      <c r="F21" s="30"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="24"/>
+      <c r="B22" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="32">
+        <v>1.8503196873457459E-2</v>
+      </c>
+      <c r="D22" s="30"/>
+      <c r="E22" s="31">
+        <v>0.94494982539930783</v>
+      </c>
+      <c r="F22" s="30"/>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="24"/>
+      <c r="B23" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="29">
+        <v>3.0545395893929017</v>
+      </c>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29">
+        <v>3.0545395893929017</v>
+      </c>
+      <c r="F23" s="29"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24" s="27"/>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="22"/>
+      <c r="C25" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="27"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="22"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="22"/>
+      <c r="B27" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="5">
+        <v>2.0516999999999999</v>
+      </c>
+      <c r="D27" s="5">
+        <v>1.9058833333333334</v>
+      </c>
+      <c r="E27" s="5">
+        <v>45.427374999999998</v>
+      </c>
+      <c r="F27" s="5">
+        <v>45.12016666666667</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="22"/>
+      <c r="B28" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="5">
+        <v>6.9741354285713639E-2</v>
+      </c>
+      <c r="D28" s="5">
+        <v>8.6876816666666742E-3</v>
+      </c>
+      <c r="E28" s="5">
+        <v>5.6098553571428435E-2</v>
+      </c>
+      <c r="F28" s="5">
+        <v>0.23225576666666661</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="22"/>
+      <c r="B29" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="5">
+        <v>8</v>
+      </c>
+      <c r="D29" s="5">
+        <v>6</v>
+      </c>
+      <c r="E29" s="5">
+        <v>8</v>
+      </c>
+      <c r="F29" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="22"/>
+      <c r="B30" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="5">
+        <v>0</v>
+      </c>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5">
+        <v>0</v>
+      </c>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="22"/>
+      <c r="B31" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" s="5">
+        <v>9</v>
+      </c>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5">
+        <v>7</v>
+      </c>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="22"/>
+      <c r="B32" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="5">
+        <v>1.4462398066860225</v>
+      </c>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5">
+        <v>1.4367202647576442</v>
+      </c>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="22"/>
+      <c r="B33" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="16">
+        <v>0.18202015937732566</v>
+      </c>
+      <c r="D33" s="5"/>
+      <c r="E33" s="16">
+        <v>0.19394736803401116</v>
+      </c>
+      <c r="F33" s="5"/>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="22"/>
+      <c r="B34" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="2">
+        <v>3.2498355415921263</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2">
+        <v>3.4994832973504946</v>
+      </c>
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35" s="28"/>
+      <c r="E35" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="F35" s="28"/>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="24"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="28"/>
+      <c r="E36" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" s="28"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="24"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="24"/>
+      <c r="B38" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="12">
+        <v>1.1410549999999999</v>
+      </c>
+      <c r="D38" s="12">
+        <v>1.0436799999999999</v>
+      </c>
+      <c r="E38" s="12">
+        <v>44.041499999999999</v>
+      </c>
+      <c r="F38" s="12">
+        <v>44.195999999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="24"/>
+      <c r="B39" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="12">
+        <v>0.1980164957666668</v>
+      </c>
+      <c r="D39" s="12">
+        <v>6.3466046400000087E-2</v>
+      </c>
+      <c r="E39" s="12">
+        <v>0.25067366666666552</v>
+      </c>
+      <c r="F39" s="12">
+        <v>0.28680100000000192</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="24"/>
+      <c r="B40" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="12">
+        <v>4</v>
+      </c>
+      <c r="D40" s="12">
+        <v>3</v>
+      </c>
+      <c r="E40" s="12">
+        <v>4</v>
+      </c>
+      <c r="F40" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="24"/>
+      <c r="B41" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" s="12">
+        <v>0</v>
+      </c>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12">
+        <v>0</v>
+      </c>
+      <c r="F41" s="12"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="24"/>
+      <c r="B42" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="12">
+        <v>5</v>
+      </c>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12">
+        <v>4</v>
+      </c>
+      <c r="F42" s="12"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="24"/>
+      <c r="B43" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C43" s="12">
+        <v>0.36632138664652431</v>
+      </c>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12">
+        <v>-0.38835678540919727</v>
+      </c>
+      <c r="F43" s="12"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="24"/>
+      <c r="B44" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C44" s="16">
+        <v>0.72911511459075773</v>
+      </c>
+      <c r="D44" s="12"/>
+      <c r="E44" s="16">
+        <v>0.71753608203899089</v>
+      </c>
+      <c r="F44" s="12"/>
+    </row>
+    <row r="45" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="24"/>
+      <c r="B45" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45" s="10">
+        <v>4.0321429835552278</v>
+      </c>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10">
+        <v>4.604094871349993</v>
+      </c>
+      <c r="F45" s="10"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B46" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D46" s="27"/>
+      <c r="E46" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="F46" s="27"/>
+    </row>
+    <row r="47" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="22"/>
+      <c r="C47" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D47" s="27"/>
+      <c r="E47" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F47" s="27"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="22"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="22"/>
+      <c r="B49" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" s="5">
+        <v>4.7075666666666676</v>
+      </c>
+      <c r="D49" s="5">
+        <v>3.8046333333333333</v>
+      </c>
+      <c r="E49" s="5">
+        <v>45.49666666666667</v>
+      </c>
+      <c r="F49" s="5">
+        <v>45.439</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="22"/>
+      <c r="B50" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50" s="5">
+        <v>3.8155833333333384E-3</v>
+      </c>
+      <c r="D50" s="5">
+        <v>1.5670643333333355E-2</v>
+      </c>
+      <c r="E50" s="5">
+        <v>1.9205333333333824E-2</v>
+      </c>
+      <c r="F50" s="5">
+        <v>1.2669999999999279E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="22"/>
+      <c r="B51" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" s="5">
+        <v>3</v>
+      </c>
+      <c r="D51" s="5">
+        <v>3</v>
+      </c>
+      <c r="E51" s="5">
+        <v>3</v>
+      </c>
+      <c r="F51" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="22"/>
+      <c r="B52" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52" s="5">
+        <v>0</v>
+      </c>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5">
+        <v>0</v>
+      </c>
+      <c r="F52" s="5"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="22"/>
+      <c r="B53" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C53" s="5">
+        <v>3</v>
+      </c>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5">
+        <v>2</v>
+      </c>
+      <c r="F53" s="5"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="22"/>
+      <c r="B54" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C54" s="5">
+        <v>11.203466977299996</v>
+      </c>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5">
+        <v>0.69807454781829215</v>
+      </c>
+      <c r="F54" s="5"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="22"/>
+      <c r="B55" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C55" s="26">
+        <v>1.5243881012774877E-3</v>
+      </c>
+      <c r="D55" s="5"/>
+      <c r="E55" s="16">
+        <v>0.55737390532056452</v>
+      </c>
+      <c r="F55" s="5"/>
+    </row>
+    <row r="56" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="22"/>
+      <c r="B56" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C56" s="2">
+        <v>5.8409093097333571</v>
+      </c>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2">
+        <v>9.9248432009182928</v>
+      </c>
+      <c r="F56" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="26">
+    <mergeCell ref="A2:A12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="A13:A23"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="A24:A34"/>
+    <mergeCell ref="A35:A45"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A46:A56"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+  </mergeCells>
+  <printOptions gridLines="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="78" fitToWidth="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;F&amp;C&amp;A</oddHeader>
+    <oddFooter>Page &amp;P of &amp;N</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>